<commit_message>
all parts here but quite messy
</commit_message>
<xml_diff>
--- a/partlist/Taobao.xlsx
+++ b/partlist/Taobao.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="378">
   <si>
     <t>Part Type</t>
   </si>
@@ -1086,9 +1086,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>470</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -1174,6 +1171,30 @@
   </si>
   <si>
     <t>POWERPAD-SOIC-8 TPS54X0</t>
+  </si>
+  <si>
+    <t>100UF-POLAR-EIA7343-10V-10%(TANT) EIA7343</t>
+  </si>
+  <si>
+    <t>capacitor, idk y this so weird</t>
+  </si>
+  <si>
+    <t>MOSFET-NCH-AO3404A SOT23-3</t>
+  </si>
+  <si>
+    <t>MOSFET-NCH-FDD8780 DPAK</t>
+  </si>
+  <si>
+    <t>CONN_07X2 2X7</t>
+  </si>
+  <si>
+    <t>DIODE-SCHOTTKY SMA-DIODE</t>
+  </si>
+  <si>
+    <t>STM32F103CBT6 LQFP48</t>
+  </si>
+  <si>
+    <t>VNH5019 POWERSO-30</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1275,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1273,6 +1294,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1631,7 +1655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1848,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D236"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C236" sqref="C236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2534,30 +2558,30 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C49" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C50" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3710,10 +3734,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B133" s="9" t="s">
         <v>342</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>343</v>
       </c>
       <c r="C133" s="9" t="s">
         <v>32</v>
@@ -4536,7 +4560,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>37</v>
@@ -4550,7 +4574,7 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>37</v>
@@ -4608,8 +4632,8 @@
       <c r="A197" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="B197" s="9" t="s">
-        <v>341</v>
+      <c r="B197" s="9">
+        <v>470</v>
       </c>
       <c r="C197" s="9" t="s">
         <v>32</v>
@@ -4634,10 +4658,10 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B199" s="9" t="s">
         <v>344</v>
-      </c>
-      <c r="B199" s="9" t="s">
-        <v>345</v>
       </c>
       <c r="C199" s="9" t="s">
         <v>32</v>
@@ -4704,7 +4728,7 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B204" s="9" t="s">
         <v>23</v>
@@ -4713,7 +4737,7 @@
         <v>34</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4844,7 +4868,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B214" s="9" t="s">
         <v>39</v>
@@ -4853,7 +4877,7 @@
         <v>39</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4872,7 +4896,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B216" s="9" t="s">
         <v>42</v>
@@ -4942,7 +4966,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B221" s="9" t="s">
         <v>45</v>
@@ -4998,7 +5022,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B225" s="9" t="s">
         <v>29</v>
@@ -5007,7 +5031,7 @@
         <v>29</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5152,16 +5176,16 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B236" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B236" s="9" t="s">
+      <c r="C236" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D236" s="9" t="s">
         <v>350</v>
-      </c>
-      <c r="C236" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="D236" s="9" t="s">
-        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -5174,159 +5198,591 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="31.9296875" customWidth="1"/>
-    <col min="3" max="3" width="24.1328125" customWidth="1"/>
+    <col min="3" max="3" width="40.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1">
+      <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="6">
+        <v>16</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="6">
+        <v>29</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="6">
+        <v>2</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="B21" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="6">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="B22" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="6">
+        <v>8</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="6">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="6">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="6">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="6">
+        <v>3</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="6">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="6">
+        <v>2</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="6">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="B30" s="6">
+        <v>47</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="6">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+      <c r="B31" s="6">
+        <v>470</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="6">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
+      <c r="B32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="6">
+        <v>1</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="6">
+        <v>4</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="6">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="6">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="6">
+        <v>4</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="6">
+        <v>4</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="6">
+        <v>1</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="6">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C8" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>285</v>
-      </c>
-      <c r="C9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
+      <c r="B40" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="6">
+        <v>4</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="6">
+        <v>1</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="6">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
+      <c r="B43" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="6">
+        <v>1</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="6">
+        <v>1</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="6">
+        <v>4</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="6">
+        <v>5</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="6">
+        <v>1</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D48" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1"/>

</xml_diff>